<commit_message>
updated default character data
</commit_message>
<xml_diff>
--- a/django_project/wfrp/example_media/default_advanced_skills.xlsx
+++ b/django_project/wfrp/example_media/default_advanced_skills.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="57">
   <si>
     <t xml:space="preserve">character</t>
   </si>
@@ -59,6 +59,138 @@
   </si>
   <si>
     <t xml:space="preserve">Language (Battle Tongue)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SALUNDRA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Animal Care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language (Bretonnian)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore (Heraldry)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore (Reikland)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore (Warfare)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weapon_skill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melee (Fencing)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Play (Harpsichord)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOLRELLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entertain (Comedy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fellowship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore (Altdorf)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore (The Empire)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pick Lock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranged (Sling)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ballistic_skill</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sleight of Hand</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERDINAND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Channelling (Shyish)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">willpower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language (Estalian)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language (Magick)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language (Wastelander)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore (Magic)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melee (Polearm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Play (Vihuela)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AMRIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Entertain (Storytelling)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language (Eltharin)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language (Guilder)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">agility</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">strength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ELSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language (Nuln)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore (Torture)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore (Ubersreik)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lore (Witches)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melee (Brawling)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ranged (Blackpowder)</t>
   </si>
 </sst>
 </file>
@@ -68,7 +200,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -89,6 +221,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -133,8 +270,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -155,15 +296,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.41"/>
   </cols>
@@ -264,6 +405,622 @@
       </c>
       <c r="D7" s="0" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C44" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>